<commit_message>
added next subplot data
</commit_message>
<xml_diff>
--- a/data/plots.xlsx
+++ b/data/plots.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emarc\AppData\Local\GitHub\EnCours\coco\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4656384-A00F-4633-B035-FF64C157DA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCDAB3C-8EBD-473C-AABF-A7380D5E255D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{F432B298-C9D1-4D5B-A48E-4305772A811C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F432B298-C9D1-4D5B-A48E-4305772A811C}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="surveyor" sheetId="2" r:id="rId2"/>
     <sheet name="subplots" sheetId="4" r:id="rId3"/>
-    <sheet name="Feuil1" sheetId="5" r:id="rId4"/>
-    <sheet name="quadrats" sheetId="3" r:id="rId5"/>
+    <sheet name="quadrats" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
   <si>
     <t>B.1</t>
   </si>
@@ -174,40 +173,7 @@
     <t>down_left</t>
   </si>
   <si>
-    <t>up_left_x</t>
-  </si>
-  <si>
-    <t>up_left_y</t>
-  </si>
-  <si>
-    <t>,,,</t>
-  </si>
-  <si>
-    <t>up_length</t>
-  </si>
-  <si>
-    <t>down_length</t>
-  </si>
-  <si>
-    <t>right_length</t>
-  </si>
-  <si>
-    <t>calculer</t>
-  </si>
-  <si>
-    <t>interpoler</t>
-  </si>
-  <si>
-    <t>&lt;</t>
-  </si>
-  <si>
     <t>surveyor</t>
-  </si>
-  <si>
-    <t>quadrats_points</t>
-  </si>
-  <si>
-    <t>quadrats_field</t>
   </si>
   <si>
     <t>point at the up-left corner of the subplot</t>
@@ -222,7 +188,25 @@
     <t>point at the down-left corner of the subplot</t>
   </si>
   <si>
-    <t>Définition of the quadrats</t>
+    <t>next_right</t>
+  </si>
+  <si>
+    <t>next_up</t>
+  </si>
+  <si>
+    <t>next subplot to the right</t>
+  </si>
+  <si>
+    <t>next subplot to the top</t>
+  </si>
+  <si>
+    <t>quadrats</t>
+  </si>
+  <si>
+    <t>subplots</t>
+  </si>
+  <si>
+    <t>Features of the subplots</t>
   </si>
 </sst>
 </file>
@@ -281,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -295,6 +279,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,8 +373,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4DB0934F-A324-4CA3-A4C5-F304CAC7199B}" name="Tableau4" displayName="Tableau4" ref="D7:E12" totalsRowShown="0" dataDxfId="14">
-  <autoFilter ref="D7:E12" xr:uid="{4DB0934F-A324-4CA3-A4C5-F304CAC7199B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4DB0934F-A324-4CA3-A4C5-F304CAC7199B}" name="Tableau4" displayName="Tableau4" ref="D7:E14" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="D7:E14" xr:uid="{4DB0934F-A324-4CA3-A4C5-F304CAC7199B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F467FA4F-A953-401B-BB90-0BF847E3622F}" name="Column" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{5A6E9B6B-C99B-416E-AA91-DB27108C07BD}" name="Content" dataDxfId="12"/>
@@ -421,8 +406,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE1E0C32-0928-48B3-8959-7C02E17FC643}" name="Tableau49" displayName="Tableau49" ref="D14:E19" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="D14:E19" xr:uid="{DE1E0C32-0928-48B3-8959-7C02E17FC643}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE1E0C32-0928-48B3-8959-7C02E17FC643}" name="Tableau49" displayName="Tableau49" ref="D16:E21" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="D16:E21" xr:uid="{DE1E0C32-0928-48B3-8959-7C02E17FC643}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5F685793-69E3-4FFA-B24D-6A17C5F4EA9C}" name="Column" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{7638DA97-E416-48A6-99D9-6B541D87D043}" name="Content" dataDxfId="7"/>
@@ -432,8 +417,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{26C3763E-971B-483C-8015-C75C7243CEF9}" name="Tableau610" displayName="Tableau610" ref="A14:B15" totalsRowShown="0">
-  <autoFilter ref="A14:B15" xr:uid="{26C3763E-971B-483C-8015-C75C7243CEF9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{26C3763E-971B-483C-8015-C75C7243CEF9}" name="Tableau610" displayName="Tableau610" ref="A16:B17" totalsRowShown="0">
+  <autoFilter ref="A16:B17" xr:uid="{26C3763E-971B-483C-8015-C75C7243CEF9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D08C50B1-1ACC-442F-AB79-D4BF2055ED1A}" name="Sheet"/>
     <tableColumn id="2" xr3:uid="{EA72C4F4-3F33-4761-BA03-467C749F49A1}" name="Content" dataDxfId="6"/>
@@ -456,14 +441,16 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3FB01355-6FE5-4EEA-BACE-F993B5F6712E}" name="Tableau7" displayName="Tableau7" ref="A1:E10" totalsRowShown="0">
-  <autoFilter ref="A1:E10" xr:uid="{3FB01355-6FE5-4EEA-BACE-F993B5F6712E}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3FB01355-6FE5-4EEA-BACE-F993B5F6712E}" name="Tableau7" displayName="Tableau7" ref="A1:G10" totalsRowShown="0">
+  <autoFilter ref="A1:G10" xr:uid="{3FB01355-6FE5-4EEA-BACE-F993B5F6712E}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3C500887-2924-431F-A79C-1196C347B4DE}" name="subplot"/>
     <tableColumn id="2" xr3:uid="{2B6BCE3D-F273-4D52-83C3-5EA8D8A5093C}" name="up_left"/>
     <tableColumn id="3" xr3:uid="{68E60DE2-FC77-4A46-9AF2-ABE3197F2E19}" name="up_right"/>
     <tableColumn id="4" xr3:uid="{87CC494D-5176-48CF-9527-0E01B1F383F5}" name="down_right"/>
     <tableColumn id="5" xr3:uid="{0F5FE0DA-F07D-4814-8317-FBCA47A3711A}" name="down_left"/>
+    <tableColumn id="6" xr3:uid="{0C58B37B-3E68-46AD-883D-41E4D8D922F2}" name="next_right"/>
+    <tableColumn id="7" xr3:uid="{1DFC5226-C0A4-45B1-8E2C-C6AC0D10D46F}" name="next_up"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -800,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203FE5FE-F468-494C-8525-DA0649C0A6AB}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -831,7 +818,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>21</v>
@@ -890,7 +877,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -904,7 +891,7 @@
         <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -912,7 +899,7 @@
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -920,7 +907,7 @@
         <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -928,66 +915,82 @@
         <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="D13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="D14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>22</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.5">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="17" spans="1:5" ht="28.5">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="D16" t="s">
+    <row r="18" spans="1:5">
+      <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
-      <c r="D17" t="s">
+    <row r="19" spans="1:5">
+      <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
-      <c r="D18" t="s">
+    <row r="20" spans="1:5">
+      <c r="D20" t="s">
         <v>29</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="4:5">
-      <c r="D19" t="s">
+    <row r="21" spans="1:5">
+      <c r="D21" t="s">
         <v>30</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1264,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5815E3C2-2671-444A-891C-9AA48A9199E9}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1275,7 +1278,7 @@
     <col min="4" max="4" width="11.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1291,8 +1294,14 @@
       <c r="E1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>13</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>14</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>15</v>
       </c>
@@ -1343,7 +1352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>18</v>
       </c>
@@ -1359,8 +1368,11 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>19</v>
       </c>
@@ -1377,7 +1389,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>20</v>
       </c>
@@ -1394,7 +1406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>23</v>
       </c>
@@ -1410,8 +1422,14 @@
       <c r="E8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>24</v>
       </c>
@@ -1428,7 +1446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>25</v>
       </c>
@@ -1454,64 +1472,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731B5C1E-DC97-4F34-A22B-D6EBFF530CAB}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA2C0E7-3F97-4951-9A0B-CC6E981EFC7D}">
   <dimension ref="A1:E481"/>
   <sheetViews>

</xml_diff>